<commit_message>
Added Search product test
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -234,6 +234,15 @@
   </si>
   <si>
     <t>FooterTest</t>
+  </si>
+  <si>
+    <t>SearchProductTest</t>
+  </si>
+  <si>
+    <t>SearchString</t>
+  </si>
+  <si>
+    <t>Stud</t>
   </si>
 </sst>
 </file>
@@ -687,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -828,6 +837,14 @@
         <v>70</v>
       </c>
       <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -844,10 +861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1400,6 +1417,27 @@
     <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added search Part 2
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
   <si>
     <t>TCID</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>Stud</t>
+  </si>
+  <si>
+    <t>AddBundleProductTest</t>
+  </si>
+  <si>
+    <t>play-by-ear</t>
   </si>
 </sst>
 </file>
@@ -345,12 +351,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -388,7 +396,7 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -403,6 +411,8 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -696,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -845,6 +855,14 @@
         <v>71</v>
       </c>
       <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -861,10 +879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1438,6 +1456,27 @@
       </c>
       <c r="B82" s="3" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added refresh bundle page test case
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="78">
   <si>
     <t>TCID</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>play-by-ear</t>
+  </si>
+  <si>
+    <t>RefreshBundleProductTest</t>
+  </si>
+  <si>
+    <t>build-a-stack</t>
   </si>
 </sst>
 </file>
@@ -351,12 +357,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -396,7 +403,7 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -413,6 +420,7 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -706,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -863,6 +871,14 @@
         <v>74</v>
       </c>
       <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -879,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="G60" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1476,6 +1492,27 @@
         <v>3</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the failing test cases ..removed most of thread.sleep
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -914,7 +914,7 @@
   <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="12" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>39</v>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" t="s">
+      <c r="A92" s="11" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed failing test case of earning val point because product is no longer available
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -260,7 +260,7 @@
     <t>EarnVaultPointTest</t>
   </si>
   <si>
-    <t>juniper-ear-jackets-earrings</t>
+    <t>pave-sputnik-ear-jackets-earring</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
   <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Modified Place Order for new customer
Add new field in credit card information, also locator changes few
places
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="87">
   <si>
     <t>TCID</t>
   </si>
@@ -166,9 +166,6 @@
     <t>ProductName</t>
   </si>
   <si>
-    <t>ice-dog-tag-layered-pendant-necklace</t>
-  </si>
-  <si>
     <t>What's New</t>
   </si>
   <si>
@@ -232,52 +229,64 @@
     <t>378282246310005</t>
   </si>
   <si>
+    <t>Whats New</t>
+  </si>
+  <si>
+    <t>FooterTest</t>
+  </si>
+  <si>
+    <t>SearchProductTest</t>
+  </si>
+  <si>
+    <t>SearchString</t>
+  </si>
+  <si>
+    <t>Stud</t>
+  </si>
+  <si>
+    <t>AddBundleProductTest</t>
+  </si>
+  <si>
+    <t>play-by-ear</t>
+  </si>
+  <si>
+    <t>RefreshBundleProductTest</t>
+  </si>
+  <si>
+    <t>build-a-stack</t>
+  </si>
+  <si>
+    <t>EarnVaultPointTest</t>
+  </si>
+  <si>
+    <t>VaultPointWithDicountTest</t>
+  </si>
+  <si>
+    <t>VaultPointAmount</t>
+  </si>
+  <si>
+    <t>DiscountCode</t>
+  </si>
+  <si>
+    <t>BBENG</t>
+  </si>
+  <si>
+    <t>CCExpirMonth</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>CCExpirYear</t>
+  </si>
+  <si>
     <t>1234</t>
   </si>
   <si>
-    <t>Whats New</t>
-  </si>
-  <si>
-    <t>FooterTest</t>
-  </si>
-  <si>
-    <t>SearchProductTest</t>
-  </si>
-  <si>
-    <t>SearchString</t>
-  </si>
-  <si>
-    <t>Stud</t>
-  </si>
-  <si>
-    <t>AddBundleProductTest</t>
-  </si>
-  <si>
-    <t>play-by-ear</t>
-  </si>
-  <si>
-    <t>RefreshBundleProductTest</t>
-  </si>
-  <si>
-    <t>build-a-stack</t>
-  </si>
-  <si>
-    <t>EarnVaultPointTest</t>
-  </si>
-  <si>
-    <t>pave-sputnik-ear-jackets-earring</t>
-  </si>
-  <si>
-    <t>VaultPointWithDicountTest</t>
-  </si>
-  <si>
-    <t>VaultPointAmount</t>
-  </si>
-  <si>
-    <t>DiscountCode</t>
-  </si>
-  <si>
-    <t>BBENG</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>starry-avatar-cuff-bracelet</t>
   </si>
 </sst>
 </file>
@@ -405,7 +414,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -426,6 +435,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -874,7 +884,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -882,7 +892,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -890,7 +900,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -898,7 +908,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -906,7 +916,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -914,7 +924,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -922,7 +932,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -936,10 +946,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -956,7 +966,9 @@
     <col min="10" max="10" width="7.33203125" style="15" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1214,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C47" s="12"/>
     </row>
@@ -1299,7 +1311,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C58" s="12"/>
     </row>
@@ -1355,7 +1367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>3</v>
       </c>
@@ -1363,7 +1375,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>15</v>
       </c>
@@ -1371,12 +1383,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
         <v>2</v>
       </c>
@@ -1384,86 +1396,98 @@
         <v>45</v>
       </c>
       <c r="C69" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
       </c>
       <c r="E69" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" t="s">
+        <v>60</v>
+      </c>
+      <c r="G69" t="s">
+        <v>59</v>
+      </c>
+      <c r="H69" t="s">
         <v>50</v>
       </c>
-      <c r="F69" t="s">
-        <v>61</v>
-      </c>
-      <c r="G69" t="s">
-        <v>60</v>
-      </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>51</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="J69" s="15" t="s">
+      <c r="K69" t="s">
         <v>53</v>
       </c>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
+        <v>64</v>
+      </c>
+      <c r="M69" t="s">
+        <v>81</v>
+      </c>
+      <c r="N69" t="s">
+        <v>83</v>
+      </c>
+      <c r="O69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" t="s">
         <v>54</v>
-      </c>
-      <c r="L69" t="s">
-        <v>65</v>
-      </c>
-      <c r="M69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A70" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C70" t="s">
-        <v>55</v>
       </c>
       <c r="D70" t="s">
         <v>18</v>
       </c>
       <c r="E70" t="s">
+        <v>55</v>
+      </c>
+      <c r="F70" t="s">
         <v>56</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>57</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>58</v>
       </c>
-      <c r="H70" t="s">
-        <v>59</v>
-      </c>
       <c r="I70" t="s">
+        <v>61</v>
+      </c>
+      <c r="J70" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K70" t="s">
         <v>62</v>
       </c>
-      <c r="J70" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K70" t="s">
-        <v>63</v>
-      </c>
       <c r="L70" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="N70">
+        <v>2015</v>
+      </c>
+      <c r="O70" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>2</v>
       </c>
@@ -1471,32 +1495,33 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G77" s="18"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1504,7 +1529,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1512,12 +1537,12 @@
         <v>3</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1533,12 +1558,12 @@
         <v>3</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -1554,12 +1579,12 @@
         <v>3</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1575,12 +1600,12 @@
         <v>3</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -1597,10 +1622,10 @@
         <v>5</v>
       </c>
       <c r="E97" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F97" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -1608,7 +1633,7 @@
         <v>3</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>17</v>
@@ -1616,11 +1641,11 @@
       <c r="D98" t="s">
         <v>18</v>
       </c>
-      <c r="E98">
-        <v>1</v>
+      <c r="E98" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F98" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified PlaceOrder and PlaceOrderForNewCustomer
Modified PlaceOrder and PlaceOrderForNewCustomer due to Tim’s changes
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="27100" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="14340" yWindow="200" windowWidth="27100" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="82">
   <si>
     <t>TCID</t>
   </si>
@@ -161,9 +161,6 @@
     <t>ProductName</t>
   </si>
   <si>
-    <t>ice-dog-tag-layered-pendant-necklace</t>
-  </si>
-  <si>
     <t>What's New</t>
   </si>
   <si>
@@ -261,6 +258,15 @@
   </si>
   <si>
     <t>pave-sputnik-ear-jackets-earring</t>
+  </si>
+  <si>
+    <t>CCExpirMonth</t>
+  </si>
+  <si>
+    <t>CCExpirYear</t>
+  </si>
+  <si>
+    <t>starry-avatar-cuff-bracelet</t>
   </si>
 </sst>
 </file>
@@ -852,7 +858,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -860,7 +866,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -868,7 +874,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -876,7 +882,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -884,7 +890,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -892,7 +898,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -911,10 +917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -932,6 +938,7 @@
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.1640625" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1189,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="12"/>
     </row>
@@ -1274,7 +1281,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C58" s="12"/>
     </row>
@@ -1330,7 +1337,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:15">
       <c r="A65" s="12" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1345,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:15">
       <c r="A66" s="12" t="s">
         <v>15</v>
       </c>
@@ -1346,12 +1353,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:15">
       <c r="A68" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="12" t="s">
         <v>2</v>
       </c>
@@ -1359,86 +1366,98 @@
         <v>45</v>
       </c>
       <c r="C69" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
       </c>
       <c r="E69" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" t="s">
+        <v>60</v>
+      </c>
+      <c r="G69" t="s">
+        <v>59</v>
+      </c>
+      <c r="H69" t="s">
         <v>50</v>
       </c>
-      <c r="F69" t="s">
-        <v>61</v>
-      </c>
-      <c r="G69" t="s">
-        <v>60</v>
-      </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>51</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="J69" s="15" t="s">
+      <c r="K69" t="s">
         <v>53</v>
       </c>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
+        <v>64</v>
+      </c>
+      <c r="M69" t="s">
+        <v>65</v>
+      </c>
+      <c r="N69" t="s">
+        <v>79</v>
+      </c>
+      <c r="O69" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="17">
+      <c r="A70" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" t="s">
         <v>54</v>
-      </c>
-      <c r="L69" t="s">
-        <v>65</v>
-      </c>
-      <c r="M69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="17">
-      <c r="A70" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C70" t="s">
-        <v>55</v>
       </c>
       <c r="D70" t="s">
         <v>18</v>
       </c>
       <c r="E70" t="s">
+        <v>55</v>
+      </c>
+      <c r="F70" t="s">
         <v>56</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>57</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>58</v>
       </c>
-      <c r="H70" t="s">
-        <v>59</v>
-      </c>
       <c r="I70" t="s">
+        <v>61</v>
+      </c>
+      <c r="J70" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K70" t="s">
         <v>62</v>
       </c>
-      <c r="J70" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K70" t="s">
-        <v>63</v>
-      </c>
       <c r="L70" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="M70" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="M70" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="N70">
+        <v>12</v>
+      </c>
+      <c r="O70">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:15">
       <c r="A73" s="12" t="s">
         <v>2</v>
       </c>
@@ -1446,32 +1465,32 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:15">
       <c r="A74" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="A77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
+      <c r="A80" s="11" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="A78" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1479,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1487,12 +1506,12 @@
         <v>3</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1508,12 +1527,12 @@
         <v>3</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1529,12 +1548,12 @@
         <v>3</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1550,7 +1569,7 @@
         <v>3</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add updated pagination test
Add updated pagination test
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
Update Color and size test
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="460" windowWidth="20760" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="13580" yWindow="460" windowWidth="20760" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -326,6 +326,24 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>VerifyColorAndSizeTest</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Clear/Gold</t>
+  </si>
+  <si>
+    <t>pave-eternity-ring</t>
   </si>
 </sst>
 </file>
@@ -453,7 +471,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -474,6 +492,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -792,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1000,6 +1019,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1008,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:O118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1799,7 +1826,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -1807,13 +1834,48 @@
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>3</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>96</v>
       </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C117" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D117" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C118" t="s">
+        <v>104</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I118" s="15"/>
+      <c r="J118"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added add items and fixed color and size
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="460" windowWidth="20760" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="20760" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="107">
   <si>
     <t>TCID</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>pave-eternity-ring</t>
+  </si>
+  <si>
+    <t>AddItemsTest</t>
   </si>
 </sst>
 </file>
@@ -811,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1027,6 +1030,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1035,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O118"/>
+  <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1877,6 +1888,33 @@
       <c r="I118" s="15"/>
       <c r="J118"/>
     </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A120" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C121" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C122" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="cmaitri@yahoo.com"/>

</xml_diff>

<commit_message>
Modified verify an item
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="108">
   <si>
     <t>TCID</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>AddItemsTest</t>
+  </si>
+  <si>
+    <t>wishbone-bracelet</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1160,61 +1163,61 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
@@ -1224,8 +1227,11 @@
       <c r="C30" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1234,6 +1240,9 @@
       </c>
       <c r="C31" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change the product name for add item test
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="20760" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="10780" yWindow="1600" windowWidth="20760" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>wishbone-bracelet</t>
+  </si>
+  <si>
+    <t>lookinglass-drops-earrings</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1918,7 +1921,7 @@
         <v>3</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C122" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Pagination test and Sort test
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -286,9 +286,6 @@
     <t>rings</t>
   </si>
   <si>
-    <t>FilterTest</t>
-  </si>
-  <si>
     <t>whats-new</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>smilez-avatar-cuff-bracelet</t>
+  </si>
+  <si>
+    <t>SortTest</t>
   </si>
 </sst>
 </file>
@@ -820,7 +820,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1242,7 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1548,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
         <v>54</v>
@@ -1608,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
@@ -1702,7 +1702,7 @@
         <v>45</v>
       </c>
       <c r="C93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D93" t="s">
         <v>79</v>
@@ -1725,10 +1725,10 @@
         <v>66</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>67</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -1797,12 +1797,12 @@
         <v>3</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -1810,13 +1810,13 @@
         <v>2</v>
       </c>
       <c r="B108" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C108" t="s">
         <v>89</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>90</v>
-      </c>
-      <c r="D108" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -1827,15 +1827,15 @@
         <v>78</v>
       </c>
       <c r="C109" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -1851,12 +1851,12 @@
         <v>3</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
@@ -1867,10 +1867,10 @@
         <v>45</v>
       </c>
       <c r="C116" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D116" t="s">
         <v>99</v>
-      </c>
-      <c r="D116" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
@@ -1878,13 +1878,13 @@
         <v>3</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C117" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
@@ -1901,10 +1901,10 @@
         <v>2</v>
       </c>
       <c r="B120" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C120" t="s">
         <v>89</v>
-      </c>
-      <c r="C120" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
@@ -1912,10 +1912,10 @@
         <v>3</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C121" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some test cases
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rumanaafroz/Automation/BaublebarTest/src/com/baublebar/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="1600" windowWidth="20760" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="65560" windowHeight="37820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -826,13 +821,13 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -852,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -860,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -868,7 +863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -876,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -884,7 +879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -892,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -900,7 +895,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -908,7 +903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -916,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -924,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -932,7 +927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -940,7 +935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -948,7 +943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -956,7 +951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -964,7 +959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -972,7 +967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -980,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -988,7 +983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -996,7 +991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -1004,7 +999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1012,7 +1007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -1020,7 +1015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1028,7 +1023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -1036,7 +1031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -1047,6 +1042,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1054,11 +1054,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" style="3" customWidth="1"/>
@@ -1076,27 +1076,27 @@
     <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1112,12 +1112,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1139,12 +1139,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="9" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1166,61 +1166,61 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1248,27 +1248,27 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1316,14 +1316,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="13"/>
       <c r="C45" s="12"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" s="12" t="s">
         <v>2</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" s="12" t="s">
         <v>3</v>
       </c>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" s="12" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49" s="12" t="s">
         <v>3</v>
       </c>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50" s="12" t="s">
         <v>3</v>
       </c>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51" s="12" t="s">
         <v>3</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52" s="12" t="s">
         <v>3</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53" s="12" t="s">
         <v>3</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54" s="12" t="s">
         <v>3</v>
       </c>
@@ -1401,12 +1401,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3">
       <c r="A56" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57" s="12" t="s">
         <v>2</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58" s="12" t="s">
         <v>3</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="C58" s="12"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59" s="12" t="s">
         <v>3</v>
       </c>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="C59" s="12"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60" s="12" t="s">
         <v>3</v>
       </c>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="C60" s="12"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61" s="12" t="s">
         <v>3</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="C61" s="12"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62" s="12" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="C62" s="12"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3">
       <c r="A63" s="12" t="s">
         <v>3</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3">
       <c r="A64" s="12" t="s">
         <v>3</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15">
       <c r="A65" s="12" t="s">
         <v>3</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15">
       <c r="A66" s="12" t="s">
         <v>15</v>
       </c>
@@ -1494,12 +1494,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15">
       <c r="A68" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15">
       <c r="A69" s="12" t="s">
         <v>2</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="17">
       <c r="A70" s="12" t="s">
         <v>3</v>
       </c>
@@ -1593,12 +1593,12 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15">
       <c r="A72" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15">
       <c r="A73" s="12" t="s">
         <v>2</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15">
       <c r="A74" s="12" t="s">
         <v>3</v>
       </c>
@@ -1614,27 +1614,27 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15">
       <c r="A76" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15">
       <c r="A80" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -1650,12 +1650,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6">
       <c r="A84" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6">
       <c r="A85" s="12" t="s">
         <v>2</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6">
       <c r="A86" s="12" t="s">
         <v>3</v>
       </c>
@@ -1671,12 +1671,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6">
       <c r="A88" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" s="12" t="s">
         <v>2</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" s="12" t="s">
         <v>3</v>
       </c>
@@ -1692,12 +1692,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" s="12" t="s">
         <v>2</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" s="12" t="s">
         <v>3</v>
       </c>
@@ -1737,12 +1737,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>2</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>3</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -1790,12 +1790,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>2</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -1811,12 +1811,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4">
       <c r="A108" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>3</v>
       </c>
@@ -1844,12 +1844,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4">
       <c r="A112" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>3</v>
       </c>
@@ -1865,12 +1865,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10">
       <c r="A116" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>2</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>3</v>
       </c>
@@ -1900,12 +1900,12 @@
       <c r="I118" s="15"/>
       <c r="J118"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10">
       <c r="A120" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10">
       <c r="A121" t="s">
         <v>2</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -1936,6 +1936,11 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1945,8 +1950,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made bunch of changes due to website design changes(pdp + nav)
</commit_message>
<xml_diff>
--- a/src/com/baublebar/data/TestCases.xlsx
+++ b/src/com/baublebar/data/TestCases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="65560" windowHeight="37820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="113">
   <si>
     <t>TCID</t>
   </si>
@@ -257,18 +257,12 @@
     <t>EarnVaultPointTest</t>
   </si>
   <si>
-    <t>pave-sputnik-ear-jackets-earring</t>
-  </si>
-  <si>
     <t>CCExpirMonth</t>
   </si>
   <si>
     <t>CCExpirYear</t>
   </si>
   <si>
-    <t>starry-avatar-cuff-bracelet</t>
-  </si>
-  <si>
     <t>PaginationTest</t>
   </si>
   <si>
@@ -348,6 +342,24 @@
   </si>
   <si>
     <t>lookinglass-drops-earrings</t>
+  </si>
+  <si>
+    <t>Log Out</t>
+  </si>
+  <si>
+    <t>20814</t>
+  </si>
+  <si>
+    <t>21577</t>
+  </si>
+  <si>
+    <t>20379</t>
+  </si>
+  <si>
+    <t>24519</t>
+  </si>
+  <si>
+    <t>25209</t>
   </si>
 </sst>
 </file>
@@ -450,12 +462,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -498,7 +511,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -517,6 +530,7 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -817,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -993,7 +1007,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -1001,7 +1015,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -1009,7 +1023,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -1017,7 +1031,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -1025,7 +1039,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -1033,7 +1047,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -1052,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O122"/>
+  <dimension ref="A1:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1245,7 +1259,7 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1316,28 +1330,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="14" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="12"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="B46" s="13"/>
       <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C47" s="12"/>
     </row>
@@ -1346,7 +1359,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="C48" s="12"/>
     </row>
@@ -1355,7 +1368,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49" s="12"/>
     </row>
@@ -1364,7 +1377,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C50" s="12"/>
     </row>
@@ -1373,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" s="12"/>
     </row>
@@ -1381,16 +1394,17 @@
       <c r="A52" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="B52" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="12"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1398,40 +1412,39 @@
         <v>3</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="14" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="14" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C58" s="12"/>
+        <v>40</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C59" s="12"/>
     </row>
@@ -1440,7 +1453,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C60" s="12"/>
     </row>
@@ -1449,7 +1462,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C61" s="12"/>
     </row>
@@ -1458,7 +1471,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C62" s="12"/>
     </row>
@@ -1466,16 +1479,17 @@
       <c r="A63" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="B63" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:15">
@@ -1483,287 +1497,287 @@
         <v>3</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:15">
       <c r="A66" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
+      <c r="A67" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
-      <c r="A68" s="14" t="s">
+    <row r="69" spans="1:15">
+      <c r="A69" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
-      <c r="A69" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" s="3" t="s">
+    <row r="70" spans="1:15">
+      <c r="A70" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>48</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>5</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E70" t="s">
         <v>49</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F70" t="s">
         <v>60</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G70" t="s">
         <v>59</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H70" t="s">
         <v>50</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I70" t="s">
         <v>51</v>
       </c>
-      <c r="J69" s="15" t="s">
+      <c r="J70" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K70" t="s">
         <v>53</v>
       </c>
-      <c r="L69" t="s">
+      <c r="L70" t="s">
         <v>64</v>
       </c>
-      <c r="M69" t="s">
+      <c r="M70" t="s">
         <v>65</v>
       </c>
-      <c r="N69" t="s">
+      <c r="N70" t="s">
+        <v>78</v>
+      </c>
+      <c r="O70" t="s">
         <v>79</v>
       </c>
-      <c r="O69" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="17">
-      <c r="A70" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C70" t="s">
+    </row>
+    <row r="71" spans="1:15" ht="17">
+      <c r="A71" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C71" t="s">
         <v>54</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>18</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>55</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F71" t="s">
         <v>56</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G71" t="s">
         <v>57</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H71" t="s">
         <v>58</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I71" t="s">
         <v>61</v>
       </c>
-      <c r="J70" s="16" t="s">
+      <c r="J71" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K71" t="s">
         <v>62</v>
       </c>
-      <c r="L70" s="17" t="s">
+      <c r="L71" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="M70" s="3" t="s">
+      <c r="M71" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N70">
+      <c r="N71">
         <v>12</v>
       </c>
-      <c r="O70">
+      <c r="O71">
         <v>2019</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
-      <c r="A72" s="11" t="s">
+    <row r="73" spans="1:15">
+      <c r="A73" s="11" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15">
-      <c r="A73" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:15">
       <c r="A74" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15">
-      <c r="A76" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
+      <c r="A75" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="A77" s="11" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15">
-      <c r="A77" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:15">
       <c r="A78" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15">
-      <c r="A80" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="11" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="11" t="s">
+    <row r="85" spans="1:6">
+      <c r="A85" s="11" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="11" t="s">
+    <row r="89" spans="1:6">
+      <c r="A89" s="11" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="11" t="s">
+    <row r="93" spans="1:6">
+      <c r="A93" s="11" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C93" t="s">
-        <v>97</v>
-      </c>
-      <c r="D93" t="s">
-        <v>79</v>
-      </c>
-      <c r="E93" t="s">
-        <v>80</v>
-      </c>
-      <c r="F93" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" t="s">
+        <v>95</v>
+      </c>
+      <c r="D94" t="s">
         <v>78</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="E94" t="s">
+        <v>79</v>
+      </c>
+      <c r="F94" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F94" s="3" t="s">
+      <c r="D95" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F95" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="97" spans="1:4">
-      <c r="A97" t="s">
-        <v>2</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>40</v>
+      <c r="A97" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1771,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1779,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1787,144 +1801,152 @@
         <v>3</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>3</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="11" t="s">
-        <v>90</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C109" t="s">
-        <v>92</v>
-      </c>
-      <c r="D109" t="s">
-        <v>93</v>
+      <c r="A109" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C110" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D110" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:10">
-      <c r="A113" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>45</v>
+      <c r="A113" s="11" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" s="11" t="s">
-        <v>100</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="117" spans="1:10">
-      <c r="A117" t="s">
-        <v>2</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C117" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D117" t="s">
-        <v>102</v>
+      <c r="A117" s="11" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C118" t="s">
+        <v>45</v>
+      </c>
+      <c r="C118" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D118" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C119" t="s">
+        <v>102</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I119" s="15"/>
+      <c r="J119"/>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I118" s="15"/>
-      <c r="J118"/>
-    </row>
-    <row r="120" spans="1:10">
-      <c r="A120" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10">
-      <c r="A121" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C121" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C122" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C123" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>